<commit_message>
prueba ok remesa abc
</commit_message>
<xml_diff>
--- a/out_dtSociedades.xlsx
+++ b/out_dtSociedades.xlsx
@@ -70,9 +70,6 @@
     <x:t>fcabezon@diariolarioja.com;  administracionclientes@elnortedecastilla.es</x:t>
   </x:si>
   <x:si>
-    <x:t>VERDAD</x:t>
-  </x:si>
-  <x:si>
     <x:t>C009</x:t>
   </x:si>
   <x:si>
@@ -172,7 +169,7 @@
     <x:t>ABC</x:t>
   </x:si>
   <x:si>
-    <x:t>C112,C200,C242</x:t>
+    <x:t>C112,C200</x:t>
   </x:si>
   <x:si>
     <x:t>pcaballero@abc.es;gadanero@vocento.com; msantiago@abc.es; mafrias@abc.es</x:t>
@@ -212,6 +209,9 @@
   </x:si>
   <x:si>
     <x:t>scortabitarte@vocento.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>C242</x:t>
   </x:si>
   <x:si>
     <x:t>C254</x:t>
@@ -705,260 +705,260 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
         <x:v>19</x:v>
-      </x:c>
-      <x:c r="C7" s="0" t="s">
-        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:3">
       <x:c r="A8" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="B8" s="0" t="s">
+      <x:c r="C8" s="0" t="s">
         <x:v>22</x:v>
-      </x:c>
-      <x:c r="C8" s="0" t="s">
-        <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:3">
       <x:c r="A9" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
         <x:v>24</x:v>
       </x:c>
-      <x:c r="B9" s="0" t="s">
+      <x:c r="C9" s="0" t="s">
         <x:v>25</x:v>
-      </x:c>
-      <x:c r="C9" s="0" t="s">
-        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:3">
       <x:c r="A10" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="B10" s="0" t="s">
+      <x:c r="C10" s="0" t="s">
         <x:v>28</x:v>
-      </x:c>
-      <x:c r="C10" s="0" t="s">
-        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:3">
       <x:c r="A11" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
         <x:v>30</x:v>
       </x:c>
-      <x:c r="B11" s="0" t="s">
+      <x:c r="C11" s="0" t="s">
         <x:v>31</x:v>
-      </x:c>
-      <x:c r="C11" s="0" t="s">
-        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:3">
       <x:c r="A12" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="C12" s="0" t="s">
         <x:v>33</x:v>
-      </x:c>
-      <x:c r="B12" s="0" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="C12" s="0" t="s">
-        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:3">
       <x:c r="A13" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
         <x:v>35</x:v>
       </x:c>
-      <x:c r="B13" s="0" t="s">
+      <x:c r="C13" s="0" t="s">
         <x:v>36</x:v>
-      </x:c>
-      <x:c r="C13" s="0" t="s">
-        <x:v>37</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:3">
       <x:c r="A14" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="B14" s="0" t="s">
+      <x:c r="C14" s="0" t="s">
         <x:v>39</x:v>
-      </x:c>
-      <x:c r="C14" s="0" t="s">
-        <x:v>40</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:3">
       <x:c r="A15" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="C15" s="0" t="s">
         <x:v>41</x:v>
-      </x:c>
-      <x:c r="B15" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="C15" s="0" t="s">
-        <x:v>42</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:3">
       <x:c r="A16" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="C16" s="0" t="s">
         <x:v>43</x:v>
-      </x:c>
-      <x:c r="B16" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="C16" s="0" t="s">
-        <x:v>44</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:3">
       <x:c r="A17" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="B17" s="0" t="s">
         <x:v>45</x:v>
       </x:c>
-      <x:c r="B17" s="0" t="s">
+      <x:c r="C17" s="0" t="s">
         <x:v>46</x:v>
-      </x:c>
-      <x:c r="C17" s="0" t="s">
-        <x:v>47</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:3">
       <x:c r="A18" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="C18" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>33</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:3">
       <x:c r="A19" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="B19" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="C19" s="0" t="s">
         <x:v>49</x:v>
-      </x:c>
-      <x:c r="B19" s="0" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="C19" s="0" t="s">
-        <x:v>50</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:3">
       <x:c r="A20" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="B20" s="0" t="s">
         <x:v>51</x:v>
       </x:c>
-      <x:c r="B20" s="0" t="s">
+      <x:c r="C20" s="0" t="s">
         <x:v>52</x:v>
-      </x:c>
-      <x:c r="C20" s="0" t="s">
-        <x:v>53</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:3">
       <x:c r="A21" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="B21" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="C21" s="0" t="s">
         <x:v>54</x:v>
-      </x:c>
-      <x:c r="B21" s="0" t="s">
-        <x:v>54</x:v>
-      </x:c>
-      <x:c r="C21" s="0" t="s">
-        <x:v>55</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:3">
       <x:c r="A22" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="B22" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="C22" s="0" t="s">
         <x:v>56</x:v>
-      </x:c>
-      <x:c r="B22" s="0" t="s">
-        <x:v>56</x:v>
-      </x:c>
-      <x:c r="C22" s="0" t="s">
-        <x:v>57</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:3">
       <x:c r="A23" s="0" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="B23" s="0" t="s">
         <x:v>58</x:v>
       </x:c>
-      <x:c r="B23" s="0" t="s">
+      <x:c r="C23" s="0" t="s">
         <x:v>59</x:v>
-      </x:c>
-      <x:c r="C23" s="0" t="s">
-        <x:v>60</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:3">
       <x:c r="A24" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="B24" s="0" t="s">
         <x:v>61</x:v>
       </x:c>
-      <x:c r="B24" s="0" t="s">
+      <x:c r="C24" s="0" t="s">
         <x:v>62</x:v>
-      </x:c>
-      <x:c r="C24" s="0" t="s">
-        <x:v>63</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:3">
       <x:c r="A25" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="B25" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="C25" s="0" t="s">
         <x:v>64</x:v>
-      </x:c>
-      <x:c r="B25" s="0" t="s">
-        <x:v>64</x:v>
-      </x:c>
-      <x:c r="C25" s="0" t="s">
-        <x:v>65</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:3">
       <x:c r="A26" s="0" t="s">
-        <x:v>66</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="B26" s="0" t="s">
-        <x:v>66</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="C26" s="0" t="s">
-        <x:v>67</x:v>
+        <x:v>56</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:3">
       <x:c r="A27" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="B27" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="C27" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:3">
       <x:c r="A28" s="0" t="s">
-        <x:v>70</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="B28" s="0" t="s">
-        <x:v>71</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="C28" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>69</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:3">
       <x:c r="A29" s="0" t="s">
-        <x:v>72</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="B29" s="0" t="s">
-        <x:v>72</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="C29" s="0" t="s">
-        <x:v>73</x:v>
+        <x:v>59</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:3">
       <x:c r="A30" s="0" t="s">
-        <x:v>74</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="B30" s="0" t="s">
-        <x:v>74</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="C30" s="0" t="s">
         <x:v>73</x:v>
@@ -966,67 +966,78 @@
     </x:row>
     <x:row r="31" spans="1:3">
       <x:c r="A31" s="0" t="s">
-        <x:v>75</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="B31" s="0" t="s">
-        <x:v>76</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="C31" s="0" t="s">
-        <x:v>77</x:v>
+        <x:v>73</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:3">
       <x:c r="A32" s="0" t="s">
-        <x:v>78</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="B32" s="0" t="s">
-        <x:v>79</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="C32" s="0" t="s">
-        <x:v>80</x:v>
+        <x:v>77</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:3">
       <x:c r="A33" s="0" t="s">
-        <x:v>81</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="B33" s="0" t="s">
-        <x:v>81</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="C33" s="0" t="s">
-        <x:v>73</x:v>
+        <x:v>80</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:3">
       <x:c r="A34" s="0" t="s">
-        <x:v>82</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="B34" s="0" t="s">
-        <x:v>82</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="C34" s="0" t="s">
-        <x:v>83</x:v>
+        <x:v>73</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:3">
       <x:c r="A35" s="0" t="s">
-        <x:v>84</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="B35" s="0" t="s">
-        <x:v>84</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="C35" s="0" t="s">
-        <x:v>85</x:v>
+        <x:v>83</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:3">
       <x:c r="A36" s="0" t="s">
+        <x:v>84</x:v>
+      </x:c>
+      <x:c r="B36" s="0" t="s">
+        <x:v>84</x:v>
+      </x:c>
+      <x:c r="C36" s="0" t="s">
+        <x:v>85</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="37" spans="1:3">
+      <x:c r="A37" s="0" t="s">
         <x:v>86</x:v>
       </x:c>
-      <x:c r="B36" s="0" t="s">
+      <x:c r="B37" s="0" t="s">
         <x:v>86</x:v>
       </x:c>
-      <x:c r="C36" s="0" t="s">
+      <x:c r="C37" s="0" t="s">
         <x:v>87</x:v>
       </x:c>
     </x:row>

</xml_diff>